<commit_message>
Update input data sheet filename
</commit_message>
<xml_diff>
--- a/books/carbomica_progbook_AKHS_Mombasa.xlsx
+++ b/books/carbomica_progbook_AKHS_Mombasa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="53">
   <si>
     <t>Targeted to (populations)</t>
   </si>
@@ -944,8 +944,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
+      <c r="A1" s="2" t="str">
+        <f>'Program targeting'!$A$3</f>
+        <v>Recycling_WasteSegregation</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -1071,8 +1072,9 @@
       <c r="K6" s="6"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
+      <c r="A8" s="2" t="str">
+        <f>'Program targeting'!$A$4</f>
+        <v>SolarSystem_Installation</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
@@ -1198,8 +1200,9 @@
       <c r="K13" s="6"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
+      <c r="A15" s="2" t="str">
+        <f>'Program targeting'!$A$5</f>
+        <v>Efficient_Chillers_Upgrade</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
@@ -1325,8 +1328,9 @@
       <c r="K20" s="6"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
+      <c r="A22" s="2" t="str">
+        <f>'Program targeting'!$A$6</f>
+        <v>Lighting_Efficiency</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>25</v>
@@ -1452,8 +1456,9 @@
       <c r="K27" s="6"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
+      <c r="A29" s="2" t="str">
+        <f>'Program targeting'!$A$7</f>
+        <v>LowGWP_Refrigerants</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
@@ -1579,8 +1584,9 @@
       <c r="K34" s="6"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="2" t="s">
-        <v>17</v>
+      <c r="A36" s="2" t="str">
+        <f>'Program targeting'!$A$8</f>
+        <v>Hybrid_Car_Use</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>25</v>
@@ -1706,8 +1712,9 @@
       <c r="K41" s="6"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="2" t="s">
-        <v>19</v>
+      <c r="A43" s="2" t="str">
+        <f>'Program targeting'!$A$9</f>
+        <v>LowGWP_Inhalers</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>25</v>
@@ -1833,8 +1840,9 @@
       <c r="K48" s="6"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="2" t="s">
-        <v>21</v>
+      <c r="A50" s="2" t="str">
+        <f>'Program targeting'!$A$10</f>
+        <v>LowGWP_AnaestheticGases</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>25</v>
@@ -1960,8 +1968,9 @@
       <c r="K55" s="6"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="2" t="s">
-        <v>23</v>
+      <c r="A57" s="2" t="str">
+        <f>'Program targeting'!$A$11</f>
+        <v>Staff_Training_Awareness</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>25</v>

</xml_diff>